<commit_message>
finish config tests v1
</commit_message>
<xml_diff>
--- a/config_portal/examples/downloads.xlsx
+++ b/config_portal/examples/downloads.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/config_portal/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/tissue-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA266A2-578E-174C-8B3A-E0AD9B4521D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED16D19B-A4C8-6742-8D39-8562CAE7A9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="2680" windowWidth="26840" windowHeight="15940" xr2:uid="{08487E98-A1B1-174D-BAB4-8799DC10973A}"/>
   </bookViews>
   <sheets>
     <sheet name="downloads" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,47 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Block</t>
   </si>
   <si>
-    <t>P1-20C</t>
-  </si>
-  <si>
     <t>Download .xlsx</t>
   </si>
   <si>
     <t>Download the data collected in this study as an Excel spreadsheet</t>
   </si>
   <si>
-    <t>HubMAP_TMC_p1_20C_3D_protINT_May8_sorted.xlsx</t>
-  </si>
-  <si>
-    <t>Download .vti</t>
-  </si>
-  <si>
-    <t>Download the data collected in this study as a VTK file</t>
-  </si>
-  <si>
-    <t>HubMAP_TMC_p1_20C_3D_protINT_May8_sorted.vti</t>
-  </si>
-  <si>
-    <t>Download `ili spreadsheet</t>
-  </si>
-  <si>
-    <t>If you would like to visualize this data using the `ili spatial data mapping tool, open the `ili website at https://ili.ucsd.edu/, select 'Volume', and drag and drop the following two files into the viewer. Then click on the '3D' tab, and choose 'Lego' for Render Mode.</t>
-  </si>
-  <si>
-    <t>HuBMAP_ili_data10-11-24.csv</t>
-  </si>
-  <si>
-    <t>Download `ili volume file</t>
-  </si>
-  <si>
-    <t>ili_vol_template.nrrd</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -84,6 +54,12 @@
   </si>
   <si>
     <t>Desc</t>
+  </si>
+  <si>
+    <t>S1-12proteomics.xlsx</t>
+  </si>
+  <si>
+    <t>S1-12</t>
   </si>
 </sst>
 </file>
@@ -470,84 +446,62 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>